<commit_message>
Integrate Agora data for elec/RQSD
</commit_message>
<xml_diff>
--- a/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
+++ b/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
@@ -1,34 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI - units progress\InputData\elec\RQSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekte\2020\2020-04_EPS_Europe\30_Forschung_(intern)\InputData_EU28\elec\RQSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC738F8B-7D64-442A-988B-A85A7638C041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="11565"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RQSD-BRQSD" sheetId="2" r:id="rId2"/>
     <sheet name="RQSD-RQSD" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Source:</t>
   </si>
   <si>
-    <t>Each U.S. state that has an RPS defines the sources that qualify for that RPS, leading to</t>
-  </si>
-  <si>
     <t>Electricity Source</t>
   </si>
   <si>
@@ -89,18 +95,6 @@
     <t>(counting everything except fossil fuels) as our definition for the BAU case.</t>
   </si>
   <si>
-    <t>model user.  The example we include uses only wind, solar, and geothermal.</t>
-  </si>
-  <si>
-    <t>Hydro is excluded because of limited potential for new large hydro and land use impacts.</t>
-  </si>
-  <si>
-    <t>Biomass is excluded because it is not truly carbon-neutral, and it has other issues, such as</t>
-  </si>
-  <si>
-    <t>local air quality impacts and land use challenges.</t>
-  </si>
-  <si>
     <t>Nuclear is excluded because of the need to manage nuclear waste.</t>
   </si>
   <si>
@@ -117,12 +111,18 @@
   </si>
   <si>
     <t>Qualifies for RPS (Boolean)</t>
+  </si>
+  <si>
+    <t>An RPS defines the sources that qualify for RPS, leading to</t>
+  </si>
+  <si>
+    <t>model user.  The example we include uses wind, solar, hydro, biomass and geothermal.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -179,8 +179,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -271,6 +271,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -306,6 +323,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -481,85 +515,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="84.59765625" customWidth="1"/>
+    <col min="2" max="2" width="84.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -569,154 +588,154 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.59765625" customWidth="1"/>
-    <col min="2" max="2" width="22.86328125" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
       <c r="B12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <f>B2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -728,154 +747,154 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.59765625" customWidth="1"/>
-    <col min="2" max="2" width="22.86328125" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
       <c r="B12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <f>B2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>0</v>

</xml_diff>

<commit_message>
Set up RQSD to include nuclear in alternate definition
</commit_message>
<xml_diff>
--- a/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
+++ b/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekte\2020\2020-04_EPS_Europe\30_Forschung_(intern)\InputData_EU28\elec\RQSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\elec\RQSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC738F8B-7D64-442A-988B-A85A7638C041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RQSD-BRQSD" sheetId="2" r:id="rId2"/>
     <sheet name="RQSD-RQSD" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -122,7 +121,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -179,8 +178,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -196,7 +195,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -271,23 +270,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -323,23 +305,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -515,27 +480,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="84.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,40 +508,40 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -588,7 +553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -598,13 +563,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" customWidth="1"/>
+    <col min="2" max="2" width="22.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -612,7 +577,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -620,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -628,7 +593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -636,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -644,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -652,7 +617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -660,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -668,7 +633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -676,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -684,7 +649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -692,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -700,7 +665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -709,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -717,7 +682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -725,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -733,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -747,23 +712,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" customWidth="1"/>
+    <col min="2" max="2" width="22.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -771,7 +736,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -779,7 +744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -787,15 +752,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -803,7 +768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -811,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -819,7 +784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -827,7 +792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -835,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -843,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -851,7 +816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -859,7 +824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -868,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -876,7 +841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -884,7 +849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -892,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Updated elec/RQSD to match description (BAU includes nuke, boolean policy lever does not)
</commit_message>
<xml_diff>
--- a/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
+++ b/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
@@ -1,27 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\elec\RQSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\eps-eu\InputData\elec\RQSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2947672-3578-4C1A-8AC5-8D5DA9E4608A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="58575" yWindow="1995" windowWidth="27090" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RQSD-BRQSD" sheetId="2" r:id="rId2"/>
     <sheet name="RQSD-RQSD" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -121,7 +127,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -270,6 +276,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -305,6 +328,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -480,27 +520,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="84.59765625" customWidth="1"/>
+    <col min="2" max="2" width="84.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,40 +550,40 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -553,23 +595,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.59765625" customWidth="1"/>
-    <col min="2" max="2" width="22.86328125" customWidth="1"/>
+    <col min="1" max="1" width="24.6328125" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -577,7 +619,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -585,7 +627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -593,15 +635,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -609,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -617,7 +659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -625,7 +667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -633,7 +675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -641,7 +683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -649,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -657,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -665,7 +707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -674,7 +716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -682,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -690,7 +732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -698,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -712,23 +754,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.59765625" customWidth="1"/>
-    <col min="2" max="2" width="22.86328125" customWidth="1"/>
+    <col min="1" max="1" width="24.6328125" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -736,7 +778,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -744,7 +786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -752,15 +794,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -768,7 +810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -776,7 +818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -784,7 +826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -792,7 +834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -800,7 +842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -808,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -816,7 +858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -824,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -833,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -841,7 +883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -849,7 +891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -857,7 +899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Updates BRQSD -> CES
</commit_message>
<xml_diff>
--- a/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
+++ b/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\elec\RQSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\elec\RQSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC3BFDD-959C-40E7-A657-7EA10D324621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4BCF98-7965-49D2-9363-A8F171087602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31125" yWindow="5070" windowWidth="24960" windowHeight="11130" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -590,8 +590,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -985,94 +985,94 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
@@ -1840,123 +1840,93 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14:AE14" si="0">B2</f>
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2535,94 +2505,94 @@
         <v>31</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.35">
@@ -2725,94 +2695,94 @@
         <v>33</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.35">
@@ -3017,7 +2987,7 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24:AE25"/>
     </sheetView>
   </sheetViews>
@@ -5438,12 +5408,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5670,20 +5642,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{044390D6-2EC7-47F1-AF9A-70E8B29FA745}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845C71C5-F42F-4A6D-B35D-EFC0EAA73A8B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5708,12 +5681,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845C71C5-F42F-4A6D-B35D-EFC0EAA73A8B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{044390D6-2EC7-47F1-AF9A-70E8B29FA745}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>